<commit_message>
added labs to xls file
</commit_message>
<xml_diff>
--- a/lablist.xlsx
+++ b/lablist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmi041/Dropbox/work/nestleder/labarealer/ips-labmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D0CDC1-7BB2-6D4D-AB8C-2351C0AAE1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B03D47-217E-3D4A-95CF-BCD5787928B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{11EDE595-D51A-0443-B694-ABD3B272423F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="224">
   <si>
     <t>mazemap-id</t>
   </si>
@@ -622,6 +622,90 @@
   </si>
   <si>
     <t>5362_0.JPG;5362_1.JPG;5362_2.JPG</t>
+  </si>
+  <si>
+    <t>5367-5361_0.JPG;5367-5361_1.JPG;5367-5361_2.JPG</t>
+  </si>
+  <si>
+    <t>5369-5373_0.JPG;5369-5373_1.JPG;5369-5373_2.JPG</t>
+  </si>
+  <si>
+    <t>5381-5380_0.JPG;5381-5380_1.JPG;5381-5380_2.JPG</t>
+  </si>
+  <si>
+    <t>5382_0.JPG;5382_1.JPG;5382_2.JPG;5382_3.JPG</t>
+  </si>
+  <si>
+    <t>5386_0.JPG;5386_1.JPG;5386_2.JPG</t>
+  </si>
+  <si>
+    <t>5387_0.JPG;5387_1.JPG;5387_2.JPG</t>
+  </si>
+  <si>
+    <t>5467-5465_0.JPG;5467-5465_1.JPG;5467-5465_2.JPG;5467-5465_3.JPG</t>
+  </si>
+  <si>
+    <t>5480_0.JPG;5480_1.JPG</t>
+  </si>
+  <si>
+    <t>5485_0.JPG;5485_1.JPG</t>
+  </si>
+  <si>
+    <t>5484_0.JPG;5484_1.JPG</t>
+  </si>
+  <si>
+    <t>5481_0.JPG;5481_1.JPG</t>
+  </si>
+  <si>
+    <t>5482_0.JPG;5482_1.JPG</t>
+  </si>
+  <si>
+    <t>5483_0.JPG;5483_1.JPG</t>
+  </si>
+  <si>
+    <t>5486_0.JPG;5486_1.JPG;5486_2.JPG</t>
+  </si>
+  <si>
+    <t>5487_0.JPG;5487_1.JPG</t>
+  </si>
+  <si>
+    <t>5488_1.JPG</t>
+  </si>
+  <si>
+    <t>5562_0.JPG;5562_1.JPG;5562_2.JPG</t>
+  </si>
+  <si>
+    <t>S33-H5-5564</t>
+  </si>
+  <si>
+    <t>Lab/Vask</t>
+  </si>
+  <si>
+    <t>Matthias</t>
+  </si>
+  <si>
+    <t>Vask for EEG</t>
+  </si>
+  <si>
+    <t>Lab/vask</t>
+  </si>
+  <si>
+    <t>5564_0.JPG;5564_1.JPG</t>
+  </si>
+  <si>
+    <t>5582_0.JPG;5582_1.JPG</t>
+  </si>
+  <si>
+    <t>5583_0.JPG;5583_1.JPG</t>
+  </si>
+  <si>
+    <t>5584_0.JPG;5584_1.JPG</t>
+  </si>
+  <si>
+    <t>5585_0.JPG;5585_1.JPG</t>
+  </si>
+  <si>
+    <t>5586_0.JPG;5586_1.JPG;5586_2.JPG;5586_3.JPG; 5586-5588_1.JPG;5586-5588_2.JPG</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0781B593-D21A-BE46-8FC7-AE3C2C393564}">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1248,7 @@
         <v>26</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1193,7 +1277,7 @@
         <v>28</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1456,7 +1540,7 @@
         <v>62</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -1485,7 +1569,7 @@
         <v>66</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>15</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1514,7 +1598,7 @@
         <v>69</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1543,7 +1627,7 @@
         <v>72</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>15</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1572,7 +1656,7 @@
         <v>72</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>15</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1601,7 +1685,7 @@
         <v>72</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>15</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1630,7 +1714,7 @@
         <v>72</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1658,9 +1742,6 @@
       <c r="I22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1887,7 +1968,7 @@
         <v>97</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1916,7 +1997,7 @@
         <v>100</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1972,7 +2053,7 @@
         <v>106</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2055,7 +2136,7 @@
         <v>114</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2084,7 +2165,7 @@
         <v>117</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>15</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2200,7 +2281,7 @@
         <v>130</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2229,7 +2310,7 @@
         <v>132</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2258,7 +2339,7 @@
         <v>135</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>15</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2287,7 +2368,7 @@
         <v>137</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>15</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2519,7 +2600,7 @@
         <v>155</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2691,7 +2772,7 @@
         <v>172</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -2720,7 +2801,7 @@
         <v>175</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -2749,7 +2830,7 @@
         <v>178</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>15</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -2778,7 +2859,7 @@
         <v>181</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>15</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2807,7 +2888,7 @@
         <v>184</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2836,7 +2917,7 @@
         <v>187</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -2890,7 +2971,30 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J66" s="3"/>
+      <c r="A66" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="1">
+        <v>5564</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J67" s="3"/>

</xml_diff>